<commit_message>
working deployable copy. templates need to be fleshed out. application.py has been fully debugged and should be ready to go.
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="190">
   <si>
     <t>race</t>
   </si>
@@ -66,16 +66,31 @@
     <t>Student Government</t>
   </si>
   <si>
+    <t>Student Government is the official student voice to the UT administration, the Board of Regents and the Texas Legislature. SG aims to represent students' interests, increase student decision-making power and improve campus life by creating effective student services.</t>
+  </si>
+  <si>
     <t>Graduate Student Assembly</t>
   </si>
   <si>
+    <t>Graduate Student Assembly is the official graduate student voice to the UT administration, the Board of Regents and the Texas Legislature. Members of the organization formally address specific graduate student concerns.</t>
+  </si>
+  <si>
     <t>University Co-Op</t>
   </si>
   <si>
+    <t>The University Unions Board of Directors recommends rules and procedures for the operation of the Unions' facilities, which include the Texas Union, the Student Activity Center and the Hogg Auditorium. The board also oversees Campus Events and Entertainment.</t>
+  </si>
+  <si>
     <t>Texas Union</t>
   </si>
   <si>
+    <t>The University Co-op Board of Directors directs the University Co-op and oversees scholarships, grants and funding. The student body elects two full-time students to serve on the board for two years.</t>
+  </si>
+  <si>
     <t>Texas Student Media</t>
+  </si>
+  <si>
+    <t>The Texas Student Media Board of Operating Trustees oversees the University's five official media outlets: KVRX 91.7 FM, the Texas Travesty, Texas Student Television, the Cactus yearbook and The Daily Texan.</t>
   </si>
   <si>
     <t>Name</t>
@@ -683,13 +698,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -757,25 +772,40 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -804,755 +834,755 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
+      <c r="A7" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
+      <c r="A8" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
+      <c r="A9" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>25</v>
+      <c r="A10" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
+      <c r="A12" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
+      <c r="A13" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
+      <c r="A14" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
+      <c r="A15" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>32</v>
+      <c r="A17" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
+      <c r="A18" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
+      <c r="A19" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>35</v>
+      <c r="A20" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>36</v>
+      <c r="A21" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>37</v>
+      <c r="A22" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>38</v>
+      <c r="A23" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>45</v>
+      <c r="A27" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>46</v>
+      <c r="A28" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>47</v>
+      <c r="A29" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>48</v>
+      <c r="A30" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>50</v>
+      <c r="A32" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>51</v>
+      <c r="A33" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>52</v>
+      <c r="A34" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="s">
-        <v>71</v>
+      <c r="A47" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
-        <v>72</v>
+      <c r="A48" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="s">
-        <v>73</v>
+      <c r="A49" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="s">
-        <v>74</v>
+      <c r="A50" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
-        <v>76</v>
+      <c r="A52" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
-        <v>77</v>
+      <c r="A53" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="s">
-        <v>78</v>
+      <c r="A54" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="s">
-        <v>79</v>
+      <c r="A55" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="s">
-        <v>80</v>
+      <c r="A56" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="s">
-        <v>94</v>
+      <c r="A67" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="s">
-        <v>97</v>
+      <c r="A69" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="s">
-        <v>98</v>
+      <c r="A70" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="3" t="s">
-        <v>99</v>
+      <c r="A72" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="s">
-        <v>102</v>
+      <c r="A74" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="s">
-        <v>103</v>
+      <c r="A75" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="s">
-        <v>104</v>
+      <c r="A76" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="s">
-        <v>105</v>
+      <c r="A77" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="s">
-        <v>107</v>
+      <c r="A79" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="s">
-        <v>110</v>
+      <c r="A81" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="3" t="s">
-        <v>111</v>
+      <c r="A83" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="s">
-        <v>114</v>
+      <c r="A85" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="s">
-        <v>115</v>
+      <c r="A86" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="s">
-        <v>116</v>
+      <c r="A87" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="3" t="s">
-        <v>117</v>
+      <c r="A89" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1569,612 +1599,612 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>123</v>
+      <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="K1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
+      <c r="A3" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
+      <c r="A10" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2190,125 +2220,125 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>123</v>
+      <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="K1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="M2" s="1">
         <v>1.0</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B5" s="5"/>
       <c r="M5" s="1">
         <v>1.0</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8">
@@ -2327,55 +2357,55 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
+      <c r="A1" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>131</v>
+      <c r="J1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="N2" s="1">
         <v>2.0</v>
@@ -2383,26 +2413,26 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2418,55 +2448,55 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
+      <c r="A1" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>131</v>
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C2" s="1">
         <v>2.0</v>
@@ -2474,58 +2504,58 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1">
         <v>1.0</v>
@@ -2533,10 +2563,10 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2552,55 +2582,55 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
+      <c r="A1" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>131</v>
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
@@ -2608,10 +2638,10 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>

</xml_diff>

<commit_message>
race selector sorta-complete, needs to fix with candidates and then start building the views
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -6,7 +6,7 @@
     <sheet state="visible" name="Races" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="Master" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Student Government" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Graduate Student Association" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Graduate Student Assembly" sheetId="4" r:id="rId6"/>
     <sheet state="visible" name="Coop" sheetId="5" r:id="rId7"/>
     <sheet state="visible" name="University Unions" sheetId="6" r:id="rId8"/>
     <sheet state="visible" name="TSM" sheetId="7" r:id="rId9"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="218">
   <si>
     <t>race</t>
   </si>
@@ -63,36 +63,54 @@
     <t>description</t>
   </si>
   <si>
+    <t>url</t>
+  </si>
+  <si>
     <t>Student Government</t>
   </si>
   <si>
     <t>Student Government is the official student voice to the UT administration, the Board of Regents and the Texas Legislature. SG aims to represent students' interests, increase student decision-making power and improve campus life by creating effective student services.</t>
   </si>
   <si>
+    <t>sg</t>
+  </si>
+  <si>
     <t>Graduate Student Assembly</t>
   </si>
   <si>
     <t>Graduate Student Assembly is the official graduate student voice to the UT administration, the Board of Regents and the Texas Legislature. Members of the organization formally address specific graduate student concerns.</t>
   </si>
   <si>
+    <t>gsa</t>
+  </si>
+  <si>
     <t>University Co-Op</t>
   </si>
   <si>
     <t>The University Unions Board of Directors recommends rules and procedures for the operation of the Unions' facilities, which include the Texas Union, the Student Activity Center and the Hogg Auditorium. The board also oversees Campus Events and Entertainment.</t>
   </si>
   <si>
-    <t>Texas Union</t>
+    <t>coop</t>
+  </si>
+  <si>
+    <t>University Union</t>
   </si>
   <si>
     <t>The University Co-op Board of Directors directs the University Co-op and oversees scholarships, grants and funding. The student body elects two full-time students to serve on the board for two years.</t>
   </si>
   <si>
+    <t>union</t>
+  </si>
+  <si>
     <t>Texas Student Media</t>
   </si>
   <si>
     <t>The Texas Student Media Board of Operating Trustees oversees the University's five official media outlets: KVRX 91.7 FM, the Texas Travesty, Texas Student Television, the Cactus yearbook and The Daily Texan.</t>
   </si>
   <si>
+    <t>tsm</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -477,29 +495,13 @@
     <t>Position</t>
   </si>
   <si>
-    <t>University-Wide Representative</t>
-  </si>
-  <si>
-    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government. 
-Let’s work together to achieve the change we want to see here at the Forty Acres. Vote Alex Tayoub for University-Wide Representative. Thank you and HOOK’EM HORNS!</t>
-  </si>
-  <si>
-    <t>Help UT empower the community of students with disabilities by expanding, promoting, and encouraging opportunities in research, leadership and careers.|||Establish a book voucher system so students can get the books they need from The Co-op and instead of paying out of pocket right there, the amount gets added to their What I Owe so financial aid and scholarships can pay for it.|||Create a task force of different members of the student body, faculty, and staff to create discussion, and come up with a variety of solutions regarding the issue of sexual assault/violence.||| Establish a more affordable meal plan for both on-campus and off-campus students.|||Make printing FREE.</t>
-  </si>
-  <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>@tayoub4uwr</t>
-  </si>
-  <si>
-    <t>http://www.facebook.com/alxtayoub</t>
+    <t>URL</t>
   </si>
   <si>
     <t>Daniel James Chapman &amp; Austin James Robinson</t>
+  </si>
+  <si>
+    <t>exec</t>
   </si>
   <si>
     <t>Jonathan Dror &amp; Delisa Shannon</t>
@@ -539,10 +541,41 @@
     <t>Kevin Helgren &amp; Binna Kim</t>
   </si>
   <si>
+    <t>University-Wide Representative</t>
+  </si>
+  <si>
+    <t>uwide</t>
+  </si>
+  <si>
+    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government. 
+Let’s work together to achieve the change we want to see here at the Forty Acres. Vote Alex Tayoub for University-Wide Representative. Thank you and HOOK’EM HORNS!</t>
+  </si>
+  <si>
+    <t>Help UT empower the community of students with disabilities by expanding, promoting, and encouraging opportunities in research, leadership and careers.|||Establish a book voucher system so students can get the books they need from The Co-op and instead of paying out of pocket right there, the amount gets added to their What I Owe so financial aid and scholarships can pay for it.|||Create a task force of different members of the student body, faculty, and staff to create discussion, and come up with a variety of solutions regarding the issue of sexual assault/violence.||| Establish a more affordable meal plan for both on-campus and off-campus students.|||Make printing FREE.</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Freshman</t>
+  </si>
+  <si>
+    <t>@tayoub4uwr</t>
+  </si>
+  <si>
+    <t>http://www.facebook.com/alxtayoub</t>
+  </si>
+  <si>
     <t>Architecture Representative</t>
   </si>
   <si>
+    <t>arch</t>
+  </si>
+  <si>
     <t>McCombs Representative</t>
+  </si>
+  <si>
+    <t>mccombs</t>
   </si>
   <si>
     <t>Ramanika Upneja</t>
@@ -562,12 +595,21 @@
     <t>Communications Representative</t>
   </si>
   <si>
+    <t>comm</t>
+  </si>
+  <si>
     <t>Education School Representative</t>
   </si>
   <si>
+    <t>edu</t>
+  </si>
+  <si>
     <t>Engineering School Representative</t>
   </si>
   <si>
+    <t>engineering</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jacob Read </t>
   </si>
   <si>
@@ -577,33 +619,57 @@
     <t>Fine Arts Representative</t>
   </si>
   <si>
+    <t>fa</t>
+  </si>
+  <si>
     <t>Geosciences School Representative</t>
   </si>
   <si>
+    <t>geo</t>
+  </si>
+  <si>
     <t>Graduate At-Large Representative</t>
   </si>
   <si>
+    <t>gradatlarge</t>
+  </si>
+  <si>
     <t>Law School Representative</t>
   </si>
   <si>
+    <t>law</t>
+  </si>
+  <si>
     <t>Liberal Arts Representative</t>
   </si>
   <si>
+    <t>cola</t>
+  </si>
+  <si>
     <t>Alexendra Thomas</t>
   </si>
   <si>
     <t>Natural Sciences Representative</t>
   </si>
   <si>
+    <t>cns</t>
+  </si>
+  <si>
     <t>Nursing School Representative</t>
   </si>
   <si>
     <t>Social Work School Representative</t>
   </si>
   <si>
+    <t>sw</t>
+  </si>
+  <si>
     <t>School of Undergraduate Studies Representative</t>
   </si>
   <si>
+    <t>ugs</t>
+  </si>
+  <si>
     <t>Number of Positions</t>
   </si>
   <si>
@@ -619,6 +685,9 @@
     <t>President</t>
   </si>
   <si>
+    <t>gsapres</t>
+  </si>
+  <si>
     <t>Michael Scott</t>
   </si>
   <si>
@@ -631,16 +700,31 @@
     <t>Vice-President</t>
   </si>
   <si>
+    <t>gsavp</t>
+  </si>
+  <si>
     <t>Board of Directors</t>
   </si>
   <si>
+    <t>board</t>
+  </si>
+  <si>
     <t xml:space="preserve">J. Dylan Adkins, McCombs School of Business </t>
   </si>
   <si>
     <t xml:space="preserve">Board of Directors </t>
   </si>
   <si>
+    <t>pres</t>
+  </si>
+  <si>
     <t>Daily Texan Editor-InChief</t>
+  </si>
+  <si>
+    <t>eic</t>
+  </si>
+  <si>
+    <t>tsmboard</t>
   </si>
 </sst>
 </file>
@@ -708,10 +792,10 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -767,45 +851,63 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -834,755 +936,755 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="4" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1600,611 +1702,848 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>140</v>
+      <c r="A2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>140</v>
+      <c r="A3" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>140</v>
+      <c r="A4" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="M22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>155</v>
-      </c>
       <c r="M23" s="1" t="s">
-        <v>18</v>
+        <v>157</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>156</v>
+        <v>165</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>53</v>
+      <c r="A25" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
+      <c r="A26" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
-        <v>51</v>
+      <c r="A27" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>57</v>
+      <c r="A28" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>54</v>
+      <c r="A29" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
-        <v>56</v>
+      <c r="A30" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5" t="s">
-        <v>52</v>
+      <c r="A32" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="s">
-        <v>61</v>
+      <c r="A34" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="s">
-        <v>60</v>
+      <c r="A35" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="s">
-        <v>64</v>
+      <c r="A37" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="7" t="s">
-        <v>62</v>
+      <c r="A38" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>163</v>
+        <v>175</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="s">
-        <v>165</v>
+      <c r="A40" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
-        <v>69</v>
+      <c r="A42" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>168</v>
+        <v>183</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>169</v>
+        <v>185</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>170</v>
+        <v>187</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
-        <v>78</v>
+      <c r="A47" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="5" t="s">
+      <c r="M54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="M54" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="M57" s="1" t="s">
-        <v>171</v>
+        <v>189</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="s">
-        <v>89</v>
+      <c r="A58" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5" t="s">
-        <v>90</v>
+      <c r="A59" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5" t="s">
-        <v>92</v>
+      <c r="A60" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5" t="s">
-        <v>88</v>
+      <c r="A61" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
-        <v>91</v>
+      <c r="A63" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>174</v>
+        <v>194</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>175</v>
+        <v>195</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2221,124 +2560,145 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="M2" s="1">
         <v>1.0</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>180</v>
+      <c r="N2" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>181</v>
+        <v>203</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
-        <v>182</v>
+      <c r="A3" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>181</v>
+        <v>203</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>184</v>
+      <c r="A4" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>181</v>
+        <v>203</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="A5" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="7"/>
       <c r="M5" s="1">
         <v>1.0</v>
       </c>
-      <c r="N5" s="5" t="s">
-        <v>183</v>
+      <c r="N5" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>179</v>
+        <v>202</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>111</v>
+      <c r="A7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>185</v>
+        <v>208</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="8">
@@ -2358,82 +2718,95 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>177</v>
+        <v>199</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="N2" s="1">
         <v>2.0</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>120</v>
+      <c r="A4" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>121</v>
+      <c r="A5" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="O5" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2449,124 +2822,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>107</v>
+      <c r="A2" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="C2" s="1">
         <v>2.0</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>109</v>
+      <c r="A3" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>110</v>
+      <c r="A4" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>112</v>
+      <c r="A5" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>108</v>
+      <c r="A6" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>111</v>
+      <c r="A7" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
-        <v>115</v>
+      <c r="A9" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1">
         <v>1.0</v>
       </c>
+      <c r="O9" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2583,68 +2986,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
routing complete. migrated all detection to front end to deal w hashes. check FIXME
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -54,6 +54,22 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D1">
+      <text>
+        <t xml:space="preserve">INSTEAD OF USING ||| PLEASE BREAK EACH LINE WITH &lt;br&gt;
+	-Jun Tan</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="218">
   <si>
@@ -510,32 +526,32 @@
     <t xml:space="preserve">Kallen Dimitroff &amp; Jesse Guadiana </t>
   </si>
   <si>
-    <t xml:space="preserve">We are Dimitroff- Guadiana and we are running to be your Student Body President and Vice President! 
-All little about us: 
-Kallen Dimitroff is a fourth year from Houston, TX. She has served the University through SG as a First Year, Liberal Arts and University-Wide Representative. She has worked on initiatives ranging from securing funding for the protected bike lane on the drag to getting students more time to pay off their financial bars during registration. She is passionate about the university and has a track record of getting things done for students. 
-Jesse Guadiana is a fourth year from Irving, TX. Jesse has spent his time on campus in the Multicultural Engagement Center as a member and executive officer in the Latino Community Affairs agency. As an Orientation Advisor and mentor to younger students Jesse has found his passion in advocating for underrepresented communities. 
-A little about the campaign: 
-We have been working for months to build a campaign worth believing in. Though our supporters come from different backgrounds we are all united around the idea that Student Government needs to improve for the betterment of the university. We believe more perspectives need to be brought into the legislative assembly room on Tuesday nights. We also believe that SG needs to spend more time working on issues that impact students and their daily lives. 
-Our platform consists of 6 points: 
-Free Transcripts 
-Affordable Housing
-Resources for First Generation Students
-Break UT’s Aramark Contract
-Better Parties
-Supporting Survivors of Sexual Assault.
+    <t xml:space="preserve">We are Dimitroff-Guadiana and we are running to be your Student Body President and Vice President!&lt;br&gt;
+A little about us:&lt;br&gt;
+Kallen Dimitroff is a fourth year from Houston, TX. She has served the University through SG as a First Year, Liberal Arts and University-Wide Representative. She has worked on initiatives ranging from securing funding for the protected bike lane on the drag to getting students more time to pay off their financial bars during registration. She is passionate about the university and has a track record of getting things done for students.&lt;br&gt;
+Jesse Guadiana is a fourth year from Irving, TX. Jesse has spent his time on campus in the Multicultural Engagement Center as a member and executive officer in the Latino Community Affairs agency. As an Orientation Advisor and mentor to younger students Jesse has found his passion in advocating for underrepresented communities.&lt;br&gt;
+A little about the campaign:&lt;br&gt; 
+We have been working for months to build a campaign worth believing in. Though our supporters come from different backgrounds we are all united around the idea that Student Government needs to improve for the betterment of the university. We believe more perspectives need to be brought into the legislative assembly room on Tuesday nights. We also believe that SG needs to spend more time working on issues that impact students and their daily lives.&lt;br&gt; 
+Our platform consists of 6 points: &lt;br&gt;
+1. Free Transcripts &lt;br&gt;
+2. Affordable Housing&lt;br&gt;
+3. Resources for First Generation Students&lt;br&gt;
+4. Break UT’s Aramark Contract&lt;br&gt;
+5. Better Parties&lt;br&gt;
+6. Supporting Survivors of Sexual Assault.&lt;br&gt;
 Each point is researched, actionable and most importantly - possible. To get more information on the points or learn more about the campaign check out our Facebook page and website: www.dimitroffguadiana.com.  We sincerely hope you decided to #RunWithUs! </t>
   </si>
   <si>
-    <t xml:space="preserve">Free transcripts|||A camp for 1st generations college students|||A permanent endowment for Voice Against Violence's Survivor's Fund|||Break UT's contract with Aramark|||Overturn city sounds ordinances to have live music in residential areas|||Sustainable Housing Affordability </t>
-  </si>
-  <si>
-    <t>History/Government|||Latin American Studies/Government</t>
+    <t xml:space="preserve">Free transcripts&lt;br&gt;A camp for 1st generation college students&lt;br&gt;A permanent endowment for Voice Against Violence's Survivor's Fund&lt;br&gt;Break UT's contract with Aramark&lt;br&gt;Overturn city sounds ordinances to have live music in residential areas&lt;br&gt;Sustainable Housing Affordability </t>
+  </si>
+  <si>
+    <t>History/Government&lt;br&gt;Latin American Studies/Government</t>
   </si>
   <si>
     <t>Seniors</t>
   </si>
   <si>
-    <t>www.dimitroffguadiana.com</t>
+    <t>http://www.dimitroffguadiana.com</t>
   </si>
   <si>
     <t>Kevin Helgren &amp; Binna Kim</t>
@@ -547,11 +563,11 @@
     <t>uwide</t>
   </si>
   <si>
-    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government. 
+    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government.&lt;br&gt;
 Let’s work together to achieve the change we want to see here at the Forty Acres. Vote Alex Tayoub for University-Wide Representative. Thank you and HOOK’EM HORNS!</t>
   </si>
   <si>
-    <t>Help UT empower the community of students with disabilities by expanding, promoting, and encouraging opportunities in research, leadership and careers.|||Establish a book voucher system so students can get the books they need from The Co-op and instead of paying out of pocket right there, the amount gets added to their What I Owe so financial aid and scholarships can pay for it.|||Create a task force of different members of the student body, faculty, and staff to create discussion, and come up with a variety of solutions regarding the issue of sexual assault/violence.||| Establish a more affordable meal plan for both on-campus and off-campus students.|||Make printing FREE.</t>
+    <t>Help UT empower the community of students with disabilities by expanding, promoting, and encouraging opportunities in research, leadership and careers.&lt;br&gt;Establish a book voucher system so students can get the books they need from The Co-op and instead of paying out of pocket right there, the amount gets added to their What I Owe so financial aid and scholarships can pay for it.&lt;br&gt;Create a task force of different members of the student body, faculty, and staff to create discussion, and come up with a variety of solutions regarding the issue of sexual assault/violence.&lt;br&gt; Establish a more affordable meal plan for both on-campus and off-campus students.&lt;br&gt;Make printing FREE.</t>
   </si>
   <si>
     <t>Economics</t>
@@ -585,7 +601,7 @@
 Currently, I serve in UT Senate and the Undergraduate Business Council because I believe that an active student voice is imperative for to maintain and encourage a successful learning environment. Thus, I hope to push our collective concerns and ideas at a university-wide level because I deeply care about student life issues at McCombs and across the University. Thank you, and I appreciate your support! #TuForYou</t>
   </si>
   <si>
-    <t>To work alongside the Undergraduate Business Council and Student Government and improve the McCombs printing maintenance problem to ensure that students can utilize services like other colleges on campus.||| To work alongside the Undergraduate Business Council and Student Government and increase much needed support and services for students pursuing entrepreneurship opportunities in Austin and beyond.
+    <t>To work alongside the Undergraduate Business Council and Student Government and improve the McCombs printing maintenance problem to ensure that students can utilize services like other colleges on campus.&lt;br&gt; To work alongside the Undergraduate Business Council and Student Government and increase much needed support and services for students pursuing entrepreneurship opportunities in Austin and beyond.
 </t>
   </si>
   <si>
@@ -718,7 +734,7 @@
     <t>pres</t>
   </si>
   <si>
-    <t>Daily Texan Editor-InChief</t>
+    <t>Daily Texan Editor-In-Chief</t>
   </si>
   <si>
     <t>eic</t>
@@ -731,7 +747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -747,6 +763,11 @@
       <sz val="12.0"/>
     </font>
     <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -775,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -793,6 +814,12 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1793,22 +1820,22 @@
         <v>150</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>153</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>154</v>
       </c>
       <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="8" t="s">
         <v>155</v>
       </c>
       <c r="K4" s="6"/>
@@ -1883,7 +1910,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>49</v>
       </c>
       <c r="M8" s="1" t="s">
@@ -1894,7 +1921,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="1" t="s">
@@ -1905,7 +1932,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>45</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -1916,7 +1943,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="9" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -1938,7 +1965,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
       <c r="M13" s="1" t="s">
@@ -1960,7 +1987,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>39</v>
       </c>
       <c r="M15" s="1" t="s">
@@ -1971,7 +1998,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
       <c r="M16" s="1" t="s">
@@ -1982,7 +2009,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -1993,7 +2020,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>44</v>
       </c>
       <c r="M18" s="1" t="s">
@@ -2004,7 +2031,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -2015,7 +2042,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
       <c r="M20" s="1" t="s">
@@ -2026,7 +2053,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>33</v>
       </c>
       <c r="M21" s="1" t="s">
@@ -2037,7 +2064,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="M22" s="1" t="s">
@@ -2048,7 +2075,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
       <c r="M23" s="1" t="s">
@@ -2070,7 +2097,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="9" t="s">
         <v>59</v>
       </c>
       <c r="M25" s="1" t="s">
@@ -2081,7 +2108,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="9" t="s">
         <v>56</v>
       </c>
       <c r="M26" s="1" t="s">
@@ -2092,7 +2119,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="9" t="s">
         <v>57</v>
       </c>
       <c r="M27" s="1" t="s">
@@ -2103,7 +2130,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="9" t="s">
         <v>63</v>
       </c>
       <c r="M28" s="1" t="s">
@@ -2114,7 +2141,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M29" s="1" t="s">
@@ -2125,7 +2152,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
         <v>62</v>
       </c>
       <c r="M30" s="1" t="s">
@@ -2147,7 +2174,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="9" t="s">
         <v>58</v>
       </c>
       <c r="M32" s="1" t="s">
@@ -2158,7 +2185,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -2184,7 +2211,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>67</v>
       </c>
       <c r="M34" s="1" t="s">
@@ -2195,7 +2222,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="9" t="s">
         <v>66</v>
       </c>
       <c r="M35" s="1" t="s">
@@ -2239,7 +2266,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="10" t="s">
         <v>74</v>
       </c>
       <c r="M39" s="1" t="s">
@@ -2250,7 +2277,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="9" t="s">
         <v>179</v>
       </c>
       <c r="M40" s="1" t="s">
@@ -2272,7 +2299,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="9" t="s">
         <v>75</v>
       </c>
       <c r="M42" s="1" t="s">
@@ -2327,7 +2354,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="9" t="s">
         <v>84</v>
       </c>
       <c r="M47" s="1" t="s">
@@ -2349,7 +2376,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="9" t="s">
         <v>88</v>
       </c>
       <c r="M49" s="1" t="s">
@@ -2360,7 +2387,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="9" t="s">
         <v>87</v>
       </c>
       <c r="M50" s="1" t="s">
@@ -2371,7 +2398,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="9" t="s">
         <v>89</v>
       </c>
       <c r="M51" s="1" t="s">
@@ -2382,7 +2409,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
       <c r="M52" s="1" t="s">
@@ -2393,7 +2420,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="9" t="s">
         <v>91</v>
       </c>
       <c r="M53" s="1" t="s">
@@ -2404,7 +2431,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="9" t="s">
         <v>82</v>
       </c>
       <c r="M54" s="1" t="s">
@@ -2415,7 +2442,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="9" t="s">
         <v>90</v>
       </c>
       <c r="M55" s="1" t="s">
@@ -2426,7 +2453,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="9" t="s">
         <v>85</v>
       </c>
       <c r="M56" s="1" t="s">
@@ -2437,7 +2464,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="9" t="s">
         <v>83</v>
       </c>
       <c r="M57" s="1" t="s">
@@ -2448,7 +2475,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="9" t="s">
         <v>95</v>
       </c>
       <c r="M58" s="1" t="s">
@@ -2459,7 +2486,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="9" t="s">
         <v>96</v>
       </c>
       <c r="M59" s="1" t="s">
@@ -2470,7 +2497,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="9" t="s">
         <v>98</v>
       </c>
       <c r="M60" s="1" t="s">
@@ -2481,7 +2508,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="9" t="s">
         <v>94</v>
       </c>
       <c r="M61" s="1" t="s">
@@ -2503,7 +2530,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
       <c r="M63" s="1" t="s">
@@ -2547,7 +2574,11 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" ref="J4"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2615,7 +2646,7 @@
       <c r="M2" s="1">
         <v>1.0</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="9" t="s">
         <v>202</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -2626,12 +2657,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="B3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9" t="s">
         <v>205</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -2642,10 +2673,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="9" t="s">
         <v>207</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -2656,14 +2687,14 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="9"/>
       <c r="M5" s="1">
         <v>1.0</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="9" t="s">
         <v>206</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -2677,7 +2708,7 @@
       <c r="A6" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="9" t="s">
         <v>201</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -2688,10 +2719,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="9" t="s">
         <v>117</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -2789,7 +2820,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2800,7 +2831,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2868,7 +2899,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2882,7 +2913,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2893,7 +2924,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2904,7 +2935,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2915,7 +2946,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2926,7 +2957,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2948,7 +2979,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>121</v>
       </c>
       <c r="B9" s="1" t="s">

</xml_diff>

<commit_message>
WORKING ROUTING AND VIEWS ARE CLEARED FOR PRODUCTION THIS IS A MOMENTOUS OCCASION
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -63,6 +63,8 @@
     <comment authorId="0" ref="D1">
       <text>
         <t xml:space="preserve">INSTEAD OF USING ||| PLEASE BREAK EACH LINE WITH &lt;br&gt;
+	-Jun Tan
+EACH LINE BREAK IN THEIR TEXT SHOULD BE &lt;br&gt;&lt;br&gt;
 	-Jun Tan</t>
       </text>
     </comment>
@@ -71,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="267">
   <si>
     <t>race</t>
   </si>
@@ -514,25 +516,28 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Daniel James Chapman &amp; Austin James Robinson</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Daniel James Chapman &amp;amp; Austin James Robinson</t>
   </si>
   <si>
     <t>exec</t>
   </si>
   <si>
-    <t>Jonathan Dror &amp; Delisa Shannon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kallen Dimitroff &amp; Jesse Guadiana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are Dimitroff-Guadiana and we are running to be your Student Body President and Vice President!&lt;br&gt;
-A little about us:&lt;br&gt;
-Kallen Dimitroff is a fourth year from Houston, TX. She has served the University through SG as a First Year, Liberal Arts and University-Wide Representative. She has worked on initiatives ranging from securing funding for the protected bike lane on the drag to getting students more time to pay off their financial bars during registration. She is passionate about the university and has a track record of getting things done for students.&lt;br&gt;
-Jesse Guadiana is a fourth year from Irving, TX. Jesse has spent his time on campus in the Multicultural Engagement Center as a member and executive officer in the Latino Community Affairs agency. As an Orientation Advisor and mentor to younger students Jesse has found his passion in advocating for underrepresented communities.&lt;br&gt;
-A little about the campaign:&lt;br&gt; 
-We have been working for months to build a campaign worth believing in. Though our supporters come from different backgrounds we are all united around the idea that Student Government needs to improve for the betterment of the university. We believe more perspectives need to be brought into the legislative assembly room on Tuesday nights. We also believe that SG needs to spend more time working on issues that impact students and their daily lives.&lt;br&gt; 
-Our platform consists of 6 points: &lt;br&gt;
+    <t>Jonathan Dror &amp;amp; Delisa Shannon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kallen Dimitroff &amp;amp; Jesse Guadiana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are Dimitroff-Guadiana and we are running to be your Student Body President and Vice President!&lt;br&gt;&lt;br&gt;
+A little about us:&lt;br&gt;&lt;br&gt;
+Kallen Dimitroff is a fourth year from Houston, TX. She has served the University through SG as a First Year, Liberal Arts and University-Wide Representative. She has worked on initiatives ranging from securing funding for the protected bike lane on the drag to getting students more time to pay off their financial bars during registration. She is passionate about the university and has a track record of getting things done for students.&lt;br&gt;&lt;br&gt;
+Jesse Guadiana is a fourth year from Irving, TX. Jesse has spent his time on campus in the Multicultural Engagement Center as a member and executive officer in the Latino Community Affairs agency. As an Orientation Advisor and mentor to younger students Jesse has found his passion in advocating for underrepresented communities.&lt;br&gt;&lt;br&gt;
+A little about the campaign:&lt;br&gt;&lt;br&gt; 
+We have been working for months to build a campaign worth believing in. Though our supporters come from different backgrounds we are all united around the idea that Student Government needs to improve for the betterment of the university. We believe more perspectives need to be brought into the legislative assembly room on Tuesday nights. We also believe that SG needs to spend more time working on issues that impact students and their daily lives.&lt;br&gt;&lt;br&gt;&lt;br&gt; 
+Our platform consists of 6 points: &lt;br&gt;&lt;br&gt;
 1. Free Transcripts &lt;br&gt;
 2. Affordable Housing&lt;br&gt;
 3. Resources for First Generation Students&lt;br&gt;
@@ -542,7 +547,7 @@
 Each point is researched, actionable and most importantly - possible. To get more information on the points or learn more about the campaign check out our Facebook page and website: www.dimitroffguadiana.com.  We sincerely hope you decided to #RunWithUs! </t>
   </si>
   <si>
-    <t xml:space="preserve">Free transcripts&lt;br&gt;A camp for 1st generation college students&lt;br&gt;A permanent endowment for Voice Against Violence's Survivor's Fund&lt;br&gt;Break UT's contract with Aramark&lt;br&gt;Overturn city sounds ordinances to have live music in residential areas&lt;br&gt;Sustainable Housing Affordability </t>
+    <t>Freshman</t>
   </si>
   <si>
     <t>History/Government&lt;br&gt;Latin American Studies/Government</t>
@@ -554,7 +559,7 @@
     <t>http://www.dimitroffguadiana.com</t>
   </si>
   <si>
-    <t>Kevin Helgren &amp; Binna Kim</t>
+    <t>Kevin Helgren &amp;amp; Binna Kim</t>
   </si>
   <si>
     <t>University-Wide Representative</t>
@@ -563,20 +568,76 @@
     <t>uwide</t>
   </si>
   <si>
-    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government.&lt;br&gt;
+    <t>Student Government is in need of diversity! My goal is to fill that slot and bring forth actual representative leadership. Beyond shoring up the diversity void, I plan to actively push for a more visible legislature that actively showcases their meetings and makes a concerted effort to become more transparent to the student body. My goals in office will be as follows if elected:&lt;br&gt;&lt;br&gt;
+I will personally work within SG and the UT admin to look at affordability and housing issues.&lt;br&gt;&lt;br&gt;
+I will look into transparency issues and call for a more active role in advertising SG meetings and events. &lt;br&gt;&lt;br&gt; Finally, I want to include a wide range of opinions and ideas into legislation that comes straight from everyday students; I want to actually represent you and your ideas.&lt;br&gt;&lt;br&gt;
+I hope you come out and vote. I want to make UT great again and together we can!
+</t>
+  </si>
+  <si>
+    <t>Affordability: I want to work within SG and the UT administration on tuition increases. Affordable housing is also a priority.&lt;br&gt;&lt;br&gt;   
+Transparency: I want to reach out to the student by holding office hours and big town hall events. Making SG visible to the average student.&lt;br&gt;&lt;br&gt;   
+Diversity: I want to bring a representative voice to the assembly, I will not be a token Hispanic, but an active member.</t>
+  </si>
+  <si>
+    <t>History, Uteach-Liberal Arts</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>shlopez13</t>
+  </si>
+  <si>
+    <t>My name is Connor Madden and I am pleased to announce my candidacy for University-Wide Representative in the Student Government Assembly. Over the course of the next two weeks you’ll have the opportunity to get to know the candidates and decide who will best represent your interests as an assembly member next year. I would cherish the opportunity to serve my fellow students in this capacity and I hope you’ll give me the chance to do so. 
+I am a Plan II and Business major from Dallas, TX. Over the course of the past year I have been involved with Student Government as a Liberal Arts Representative and through the Longhorn Advocates program. I look forward to meeting many of you (if I haven’t already) through the campaigning process.
+Thanks and Hook 'Em!
+</t>
+  </si>
+  <si>
+    <t>CIVIC ENGAGEMENT- Providing students with information and resources as they arrive on campus or during orientation. This year’s general election presents a tremendous opportunity to encourage student participation and increase voter turnout. &lt;br&gt;&lt;br&gt;
+COMMUNITY SERVICE- Working with professors and administrative staff to include community service as part of their course curriculum. Promoting student leadership in the community through volunteerism and activism. 
+&lt;br&gt;&lt;br&gt;
+STUDENT HEALTH/SAFETY- Supporting initiatives that improve students’ access to and awareness of health care resources. Assisting CMHC outreach and educational efforts. Identifying areas around campus where student safety is a concern and exploring possible solutions.
+</t>
+  </si>
+  <si>
+    <t>Plan II Honors &amp;amp; Business (Management)</t>
+  </si>
+  <si>
+    <t>Sophomore</t>
+  </si>
+  <si>
+    <t>VoteMadden</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/959161137491319/</t>
+  </si>
+  <si>
+    <t>Hi Longhorns! My name is Drew Orland, and I'm a second-year Economics major from Plano, TX.&lt;br&gt;&lt;br&gt;
+I think the most important thing an SG representative can bring to the table is a thorough understanding of the student body. Through my involvement in so many different programs and organizations around campus, I have obtained a multifaceted perspective of campus that incorporates the interests of so many diverse groups of students.&lt;br&gt;&lt;br&gt;
+The thing that I believe prepares me best for SG and the thing I am most proud of from my time at UT so far is my role as Director of the Guild of Carillonneurs, playing the bells at the top of the Tower. Not just because it is so fun, but because it gives me a chance to interact with students on a daily basis in a way that produces tangible results. It's fun to go up and play fancy classical music, but my favorite part of the job is playing songs that students request. In this way I feel like I get to represent you from the top of the Tower every day, and now I'd like the chance to represent you in Student Government as well.
+Thanks, and Hook 'em Horns!
+</t>
+  </si>
+  <si>
+    <t>Connecting to the UT/Austin Community – Helping students feel at home at UT and in Austin&lt;br&gt;&lt;br&gt;  COMMUNITY SERVICE : One of the best ways to explore Austin is by volunteering with local charities and non-profits to benefit the greater Austin community. I think the university should offer more opportunities and make it easier for students to volunteer around Austin.&lt;br&gt;&lt;br&gt;  EARLY INVOLVEMENT : Because UT is such a big school, it’s often too easy for incoming students to fall through the cracks and feel like just another face in the crowd. If we push organization and program involvement more at Orientation and early on in the school year, we can make it easier for freshmen and transfer students to find a small community that makes campus feel like home.&lt;br&gt;&lt;br&gt;VOTER REGISTRATION : UT can combat the often low voter turnout of college-aged citizens by making voter registration more accessible to its students. One of the most effective ways we can make this a reality is by offering more opportunities to register as a voter in highly trafficked areas of campus and as part of programs that every student participates in, like Orientation.&lt;br&gt;&lt;br&gt;DIVERSITY AWARENESS : UT is a diverse campus in many ways, with students coming from all different kinds of backgrounds and identities. I believe the University should respect and accommodate these differences whenever possible. As your representative, I would work to make the university more LGBTQ-friendly in the way it interacts with and accommodates students. I believe the university should also do a better job addressing race-related incidents that make campus feel less welcome to minority students.</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/685701271569685/</t>
+  </si>
+  <si>
+    <t>Hello Longhorns! My name is Alex Tayoub and I’m an Economics, Pre-Med first-year running to be one of your eight University-Wide Representatives. I believe that Student Government is missing representation for the various student communities out there on the Forty Acres. Students with disabilities, transfer students, first-generation students, Hispanic students, Middle Eastern students, low-income students; these are all communities of students that I’m a part of, yet there is little to no representation of these student communities in Student Government. I want to change that. I want to bring the issues and concerns of the diverse student body to the table so that they are discussed and addressed. I want to make Student Government more accessible so that everyone can have their voice heard in Student Government.&lt;br&gt;&lt;br&gt;
 Let’s work together to achieve the change we want to see here at the Forty Acres. Vote Alex Tayoub for University-Wide Representative. Thank you and HOOK’EM HORNS!</t>
   </si>
   <si>
     <t>Help UT empower the community of students with disabilities by expanding, promoting, and encouraging opportunities in research, leadership and careers.&lt;br&gt;Establish a book voucher system so students can get the books they need from The Co-op and instead of paying out of pocket right there, the amount gets added to their What I Owe so financial aid and scholarships can pay for it.&lt;br&gt;Create a task force of different members of the student body, faculty, and staff to create discussion, and come up with a variety of solutions regarding the issue of sexual assault/violence.&lt;br&gt; Establish a more affordable meal plan for both on-campus and off-campus students.&lt;br&gt;Make printing FREE.</t>
   </si>
   <si>
-    <t>Economics</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>@tayoub4uwr</t>
+    <t>tayoub4uwr</t>
   </si>
   <si>
     <t>http://www.facebook.com/alxtayoub</t>
@@ -594,7 +655,18 @@
     <t>mccombs</t>
   </si>
   <si>
-    <t>Ramanika Upneja</t>
+    <t xml:space="preserve">To me, having a chance to represent the school that accepted me and will shape the upcoming years of my life is the best way that I can give back. If I am elected, I will bring to this position dedication to the general improvement of the campus as a whole. As a member of the Undergraduate Business Council and the Senate of College Councils, I have had the opportunity to take leadership roles in gauging the needs of students in both McCombs and around the campus. I will bring a commitment to continuing to foster a strong collaborative atmosphere between McCombs and the other schools that make up this university. I hope I prove to be a valuable asset through which the voices of students can clearly be heard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work to foster a collaborative atmosphere between McCombs and the other schools that make up this campus&lt;br&gt;&lt;br&gt;
+Ensure that minority students are able to aptly have their voices in heard in student issues concerning McCombs and the university in general&lt;br&gt;&lt;br&gt;
+Promote open and free lines of communication that includes the students, faculty, their representatives </t>
+  </si>
+  <si>
+    <t>Business (Undeclared) and Government</t>
+  </si>
+  <si>
+    <t>Dhrov &amp;quot;Drew&amp;quot; Subramanian</t>
   </si>
   <si>
     <t>Hello! My name is Vivianne Tu, and I am running for this position because I strive to strengthen the diverse, passionate, and unique voice of McCombs in our student government. McCombs students cultivate an outstanding culture of innovation, hard work, and passion, and it would be my greatest honor to serve as the bridge between the voice of McCombs students and Student Government. 
@@ -608,18 +680,56 @@
     <t>https://www.facebook.com/Tu4You</t>
   </si>
   <si>
+    <t>Ramanika Upneja</t>
+  </si>
+  <si>
     <t>Communications Representative</t>
   </si>
   <si>
     <t>comm</t>
   </si>
   <si>
+    <t xml:space="preserve">If you attend the Moody College of Communication, you are important. As a Longhorn Legislative Aide in UTSG and a member of the Communication Council, I am aware of our college’s reputation on campus. As your representative, I am ready to make decisions with you that will make our experience at Moody a better one. The time is now to have a representative who is both excited and enthusiastic about what they can do to give back to the Moody College of Communication. The decision is now yours! “Comm together” March 2 and 3 on utexasvote.org and vote for me as your Communication Representative. </t>
+  </si>
+  <si>
+    <t>1. “BMC – our open home, open longer” – If elected, I hope to adjust current facility hours at the Belo Center for New Media. My goal is to change the closing time from 11pm to 12am, during the workweek. This would give students a more comfortable option for late-night studying&lt;br&gt;&lt;br&gt;
+2. “Cappy’s Place – a place for Bevo Bucks” – We all love Cappy’s Place located in BMC, but as your representative I will increase talks on having Cappy’s Place (and more of your favorite local merchants) use the Bevo Bucks payment system&lt;br&gt;&lt;br&gt;
+3. “Moody Mentors” – a tentative idea for a program that matches Moody undergrads with “Moody Mentors” who are older than them. The mentors would either be in graduate school or in opportunities within Moody that younger students might be interested in learning more about (UTLA, Senior Fellows, or the Annette Strauss Institute are just a few examples)&lt;br&gt;&lt;br&gt;
+4. “Comm Together” – I am calling all majors and students from all backgrounds to converge together and share you ideas and visions for the Moody College of Communication with me. I cannot do this job alone. If elected, I will hold daily office hours in the Student Leadership Suite of BMC to hear your concerns!
+</t>
+  </si>
+  <si>
+    <t>Communication Studies, Corporate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freshman </t>
+  </si>
+  <si>
+    <t>votestevencomm</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/steven.santoyo</t>
+  </si>
+  <si>
     <t>Education School Representative</t>
   </si>
   <si>
     <t>edu</t>
   </si>
   <si>
+    <t>My name is Lindsey Pearlstein and I am a junior from Boston, Massachusetts, studying Applied Learning and Development (Generalist). I am currently participating in the Literacy Cohort for the Professional Development Sequence. Additionally, I am receiving a certificate in Public Policy through the Bridging Disciplines Program. I will aim to create change within the college by combining my passion for education with my interest in policy. As the College of Education Representative, I would advocate to increase diversity within the college and to expand communication between the Department of Curriculum and Instruction and the Department of Kinesiology and Health Education.
+&lt;br&gt;&lt;br&gt;
+Feel free to ask me any questions in person or by email at lindseypearlstein@utexas.edu.
+&lt;br&gt;&lt;br&gt;
+Thank you for your consideration!</t>
+  </si>
+  <si>
+    <t>Applied Learning and Development</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
     <t>Engineering School Representative</t>
   </si>
   <si>
@@ -665,21 +775,72 @@
     <t>Alexendra Thomas</t>
   </si>
   <si>
+    <t xml:space="preserve">Students attend the University of Texas for two main reasons. One is to receive an elite education in preparation for entrance into the job field. The other is to create enduring and meaningful relationships with students and faculty. As a representative of the College of Liberal Arts, I will improve both of these aspects of student life. Creating an alumni lecture series and an annual tour of the Capitol for juniors and seniors will lower concerns about finding jobs. Increasing COLA’s social media presence and forming more social events and organizations will allow students to identify peers with whom they have common interests, build study groups, and more. I have experience in leadership, extensive involvement in social life at UT, and prior familiarity with Student Government. Your vote will enable me to improve the everyday lives of hundreds of COLA students. </t>
+  </si>
+  <si>
+    <t>I would aim to provide more lectures from alumni about their careers and how they obtained success in the job field.
+&lt;br&gt;&lt;br&gt;
+I would aim to connect students to students through tailgates, social gatherings, and Facebook groups.
+&lt;br&gt;&lt;br&gt;
+I would aim to enact an annual Senior Shadow Day in which
+each incoming freshman could shadow a senior’s class day.
+&lt;br&gt;&lt;br&gt;
+I would aim to plan an annual one-day Capitol tour for juniors and seniors.</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alexandraa_7 </t>
+  </si>
+  <si>
     <t>Natural Sciences Representative</t>
   </si>
   <si>
     <t>cns</t>
   </si>
   <si>
+    <t>My name is Ramsey Hashem and I want to serve you as College of Natural Sciences Representative. During my time as a Longhorn Legislative Aide this year, I’ve attended every Student Government meeting, learning how UTSG works and working with my fellow LLAs, Representatives, and Executive Board members on various projects. I’ve gotten to see all that UTSG is capable of, including outstanding accomplishments ranging from the removal of the Jefferson Davis statue to increased support for sexual assault victims to more food trucks on campus. As Natural Sciences Representative, I want to keep doing the things that have put UT at the forefront of positive change, while reducing the disharmony that arises far too often in Student Government. My aim is to ensure that the College of Natural Sciences continues producing the influential research and making the groundbreaking discoveries that prove time and time again that CNS has some of the most innovative and brightest students at one of the best universities in the world.&lt;br&gt;&lt;br&gt; 
+I want to accomplish this in four major ways: by increasing and sustaining engagement between all of the CNS Representatives and the students they represent, supporting more intuitive course listings, educating non-CS majors about the many computer science resources online and elsewhere, and providing more opportunity for engagement between students and alumni. Above all else, I pledge to be your advocate whenever and wherever I can. I don’t want to be a faceless Representative whose name hardly anyone knows. On the contrary, I will be constantly interacting with and hearing the concerns of Natural Sciences students, no matter what the issue. If you want someone who will ensure your voice is heard, I’m the candidate who will do so and who will hold the other CNS Representatives accountable as well. 
+&lt;br&gt;&lt;br&gt;
+If I haven’t yet earned your vote, perhaps a rousing science joke will win you over: A police officer pulls Heisenberg over and asks him, “Do you know how fast you were going?” Heisenberg replies, “No, but I know where I am.” 
+&lt;br&gt;&lt;br&gt;
+Thank you so much and please don’t hesitate to reach out to me on social media, at my email (ramseyhashem@utexas.edu) or on Club Penguin. And don’t forget to vote! #Ram4CNS
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ensure more engagement between student government and the students they represent through weekly forums and updates. One of the biggest concerns I have regarding student government is the apparent disconnect between Representatives and their constituents. Too much disengagement between Student Government and the student body is occurring, and the way to start changing that dynamic is by consistently listening to the ideas of the students and by keeping them informed of Student Government activities.&lt;br&gt;&lt;br&gt;Support an easier way for students to see their degree plans and the classes they can and likely should be taking. Most students realize that they can take classes that overlap for requirements regarding a minor/certificate and that there are ways to squeeze in that spring semester in Italy or Australia, but finding out what those courses are is not as seamless as it could be. Revamping the way students see their degree plans and the courses they can (and probably should) take would allow students to more efficiently plan their schedules and would make meetings with academic advisors more productive.&lt;br&gt;&lt;br&gt;Increase access to computer science resources for non-CS majors. Having programming skills is becoming increasingly important for employers, especially for those in the sciences. Many students understand this, but unfortunately it is difficult for them to get into CS classes due to high popularity. I will support educating non-CS majors about the resources for gaining programming skills, as there are several outstanding ways to learn how to code online for free.&lt;br&gt;&lt;br&gt; Provide more opportunities for students to meet with alumni of their department. Many students at one time or another are faced with uncertainty and doubt regarding their major and career path. Having more access to alumni from a student’s same department would provide students with advice and insight from those who once tread the same path.</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>RamseyHashem</t>
+  </si>
+  <si>
     <t>Nursing School Representative</t>
   </si>
   <si>
+    <t>nursing</t>
+  </si>
+  <si>
     <t>Social Work School Representative</t>
   </si>
   <si>
     <t>sw</t>
   </si>
   <si>
+    <t xml:space="preserve">My name is Griffin Olesky and I am running to be your Undergraduate Studies Representative.  As students in UGS, we are all well aware that our time here is limited and that we have to be thinking constantly about where we want to go next. I want to make your experience in UGS as enjoyable as possible and in turn make your transition to your next school seamless. If elected, I will work closely with the Student Government, as well as the Dean of UGS, to make sure that your opinions and ideas are heard.  I often think about how lucky I am to be in UGS because, honestly, I have no idea what I want to do with my life and with this school I actually have time to think about it.  The world is my oyster and if you vote for me, it can be yours too!  </t>
+  </si>
+  <si>
+    <t>Increase transparency between Student Government and the UGS student body.&lt;br&gt;&lt;br&gt;Improve the transition process from UGS to whatever school is right for each student.&lt;br&gt;&lt;br&gt;
+Create a simple platform for UGS students to voice their opinions. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undeclared </t>
+  </si>
+  <si>
     <t>School of Undergraduate Studies Representative</t>
   </si>
   <si>
@@ -692,6 +853,9 @@
     <t>Running With</t>
   </si>
   <si>
+    <t>Michael Scott</t>
+  </si>
+  <si>
     <t>Wills Brown</t>
   </si>
   <si>
@@ -704,9 +868,6 @@
     <t>gsapres</t>
   </si>
   <si>
-    <t>Michael Scott</t>
-  </si>
-  <si>
     <t>Warner Cook</t>
   </si>
   <si>
@@ -719,25 +880,57 @@
     <t>gsavp</t>
   </si>
   <si>
+    <t xml:space="preserve">J. Dylan Adkins, McCombs School of Business </t>
+  </si>
+  <si>
     <t>Board of Directors</t>
   </si>
   <si>
     <t>board</t>
   </si>
   <si>
-    <t xml:space="preserve">J. Dylan Adkins, McCombs School of Business </t>
+    <t>As a Brand Ambassador of the Co-Op, you've seen Alexa take over the Co-Op's Snapchat and be featured on their Instagram. &lt;br&gt;&lt;br&gt;As an employee of the Co-Op, you've had Alexa help you find an item or as your cashier. 
+&lt;br&gt;&lt;br&gt;As a member of the Co-Op's Board of Directors, you'll see Alexa give your organization funding and help you get your rebate cards.
+&lt;br&gt;&lt;br&gt;Vote for Alexa! She knows the Co-Op!</t>
+  </si>
+  <si>
+    <t>Expand student knowledge about rebate cards and the opportunity for organization funding.&lt;br&gt;&lt;br&gt;Help the Co-Op become an even more influential leader as the #1 college bookstore in America.</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>http://tinyurl.com/CoOpAlexa</t>
   </si>
   <si>
     <t xml:space="preserve">Board of Directors </t>
   </si>
   <si>
-    <t>pres</t>
+    <t>unionboard</t>
+  </si>
+  <si>
+    <t>Helen Yang</t>
+  </si>
+  <si>
+    <t>unionpres</t>
   </si>
   <si>
     <t>Daily Texan Editor-In-Chief</t>
   </si>
   <si>
+    <t>My name is Alexander Chase, and I am excited to be running to be Editor-in-Chief of The Daily Texan. I will bring my experience working as a columnist and an associate editor to the position, and do my best to better every writer who comes into our office. In what promises to a tenuous year filled with hot-button issues, I will value the opinion of every student on campus, and do my best to promote an atmosphere of cooperation and understanding on campus.</t>
+  </si>
+  <si>
+    <t>Plan II, Economics</t>
+  </si>
+  <si>
+    <t>alexwchase</t>
+  </si>
+  <si>
     <t>eic</t>
+  </si>
+  <si>
+    <t>TSM Board &amp;#47; Moody College Place 2</t>
   </si>
   <si>
     <t>tsmboard</t>
@@ -796,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -826,7 +1019,13 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1723,7 +1922,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
@@ -1770,10 +1974,13 @@
       <c r="N1" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1790,12 +1997,12 @@
         <v>24</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1812,31 +2019,31 @@
         <v>24</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>150</v>
+      <c r="A4" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="7" t="s">
         <v>152</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1844,12 +2051,12 @@
         <v>24</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1866,7 +2073,7 @@
         <v>24</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6">
@@ -1874,72 +2081,60 @@
         <v>36</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N6" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="M7" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11">
@@ -1947,109 +2142,157 @@
         <v>48</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N12" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N14" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N15" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N16" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N18" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21">
@@ -2057,54 +2300,91 @@
         <v>33</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N21" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="N22" s="1" t="s">
-        <v>158</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="9" t="s">
-        <v>42</v>
+      <c r="A23" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>52</v>
+      <c r="A24" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
         <v>59</v>
       </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="M25" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26">
@@ -2112,179 +2392,211 @@
         <v>56</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>60</v>
+        <v>186</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>169</v>
+      <c r="A31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="A32" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="J32" s="1"/>
       <c r="M32" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>172</v>
+        <v>67</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="9" t="s">
-        <v>66</v>
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>64</v>
+      <c r="A36" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
-        <v>70</v>
+      <c r="A37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="s">
-        <v>68</v>
+      <c r="A38" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
-        <v>74</v>
+      <c r="A39" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41">
@@ -2292,142 +2604,142 @@
         <v>71</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="9" t="s">
-        <v>75</v>
+      <c r="A42" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>78</v>
+      <c r="A46" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>191</v>
+      <c r="A48" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54">
@@ -2435,10 +2747,10 @@
         <v>82</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55">
@@ -2446,131 +2758,162 @@
         <v>90</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="9" t="s">
-        <v>85</v>
+      <c r="A56" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="9" t="s">
-        <v>96</v>
+      <c r="A59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
-        <v>92</v>
+      <c r="A62" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>192</v>
+        <v>223</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="9" t="s">
-        <v>97</v>
+      <c r="A63" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>193</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>195</v>
+        <v>236</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="N66" s="1" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2627,10 +2970,10 @@
         <v>144</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>145</v>
@@ -2640,96 +2983,91 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="A2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M3" s="1">
         <v>1.0</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="M3" s="9"/>
       <c r="N3" s="9" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="B5" s="9"/>
       <c r="M5" s="1">
         <v>1.0</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="N7" s="9" t="s">
         <v>117</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>209</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8">
@@ -2788,35 +3126,51 @@
         <v>144</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.0" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" ht="15.0" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="B3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="N3" s="1">
         <v>2.0</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
@@ -2824,10 +3178,10 @@
         <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>250</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
@@ -2835,9 +3189,16 @@
         <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="O5" s="1"/>
+        <v>250</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="O6" s="1" t="s">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2859,7 +3220,7 @@
         <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>134</v>
@@ -2900,16 +3261,16 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="C2" s="1">
         <v>2.0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3">
@@ -2917,65 +3278,65 @@
         <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>118</v>
+      <c r="A5" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>114</v>
+      <c r="A6" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>111</v>
+      <c r="A8" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9">
@@ -2989,7 +3350,7 @@
         <v>1.0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10">
@@ -3000,7 +3361,7 @@
         <v>120</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -3023,7 +3384,7 @@
         <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>134</v>
@@ -3067,13 +3428,25 @@
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="O2" s="1" t="s">
-        <v>216</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
@@ -3081,13 +3454,13 @@
         <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>265</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>217</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>